<commit_message>
added additional sentiment analysis
</commit_message>
<xml_diff>
--- a/Excel reports/mrk_raw_dataset.xlsx
+++ b/Excel reports/mrk_raw_dataset.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G148"/>
+  <dimension ref="A1:G150"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,7 +539,7 @@
         <v>86.80343627929688</v>
       </c>
       <c r="F4" t="n">
-        <v>79.81497955322266</v>
+        <v>79.81497192382812</v>
       </c>
       <c r="G4" t="n">
         <v>45884899</v>
@@ -562,7 +562,7 @@
         <v>82.04198455810547</v>
       </c>
       <c r="F5" t="n">
-        <v>75.43685913085938</v>
+        <v>75.43687438964844</v>
       </c>
       <c r="G5" t="n">
         <v>45975656</v>
@@ -585,7 +585,7 @@
         <v>81.52671813964844</v>
       </c>
       <c r="F6" t="n">
-        <v>74.96307373046875</v>
+        <v>74.96308135986328</v>
       </c>
       <c r="G6" t="n">
         <v>49493162</v>
@@ -608,7 +608,7 @@
         <v>81.18320465087891</v>
       </c>
       <c r="F7" t="n">
-        <v>74.64723205566406</v>
+        <v>74.647216796875</v>
       </c>
       <c r="G7" t="n">
         <v>81640353</v>
@@ -631,7 +631,7 @@
         <v>78.864501953125</v>
       </c>
       <c r="F8" t="n">
-        <v>72.51519775390625</v>
+        <v>72.51519012451172</v>
       </c>
       <c r="G8" t="n">
         <v>68606796</v>
@@ -700,7 +700,7 @@
         <v>78.43511199951172</v>
       </c>
       <c r="F11" t="n">
-        <v>72.12036895751953</v>
+        <v>72.12037658691406</v>
       </c>
       <c r="G11" t="n">
         <v>85685737</v>
@@ -723,7 +723,7 @@
         <v>73.23473358154297</v>
       </c>
       <c r="F12" t="n">
-        <v>67.33866882324219</v>
+        <v>67.33868408203125</v>
       </c>
       <c r="G12" t="n">
         <v>99266351</v>
@@ -757,7 +757,7 @@
         <v>68.09160614013672</v>
       </c>
       <c r="F14" t="n">
-        <v>63.12685012817383</v>
+        <v>63.1268424987793</v>
       </c>
       <c r="G14" t="n">
         <v>106457307</v>
@@ -780,7 +780,7 @@
         <v>68.44465637207031</v>
       </c>
       <c r="F15" t="n">
-        <v>63.45415496826172</v>
+        <v>63.45415115356445</v>
       </c>
       <c r="G15" t="n">
         <v>87108502</v>
@@ -803,7 +803,7 @@
         <v>72.75763702392578</v>
       </c>
       <c r="F16" t="n">
-        <v>67.45264434814453</v>
+        <v>67.45265960693359</v>
       </c>
       <c r="G16" t="n">
         <v>65430832</v>
@@ -826,7 +826,7 @@
         <v>78.71183013916016</v>
       </c>
       <c r="F17" t="n">
-        <v>72.97272491455078</v>
+        <v>72.97271728515625</v>
       </c>
       <c r="G17" t="n">
         <v>50330514</v>
@@ -849,7 +849,7 @@
         <v>79.63740539550781</v>
       </c>
       <c r="F18" t="n">
-        <v>73.83079528808594</v>
+        <v>73.830810546875</v>
       </c>
       <c r="G18" t="n">
         <v>55249303</v>
@@ -872,7 +872,7 @@
         <v>77.70037841796875</v>
       </c>
       <c r="F19" t="n">
-        <v>72.03500366210938</v>
+        <v>72.03501892089844</v>
       </c>
       <c r="G19" t="n">
         <v>57325180</v>
@@ -918,7 +918,7 @@
         <v>72.90076446533203</v>
       </c>
       <c r="F21" t="n">
-        <v>67.58534240722656</v>
+        <v>67.58535003662109</v>
       </c>
       <c r="G21" t="n">
         <v>50060654</v>
@@ -964,7 +964,7 @@
         <v>72.87213897705078</v>
       </c>
       <c r="F23" t="n">
-        <v>67.55882263183594</v>
+        <v>67.55881500244141</v>
       </c>
       <c r="G23" t="n">
         <v>49529948</v>
@@ -1010,7 +1010,7 @@
         <v>78.49236297607422</v>
       </c>
       <c r="F25" t="n">
-        <v>72.76925659179688</v>
+        <v>72.76924896240234</v>
       </c>
       <c r="G25" t="n">
         <v>51003959</v>
@@ -1033,7 +1033,7 @@
         <v>72.80534362792969</v>
       </c>
       <c r="F26" t="n">
-        <v>67.49687957763672</v>
+        <v>67.49688720703125</v>
       </c>
       <c r="G26" t="n">
         <v>59188420</v>
@@ -1090,7 +1090,7 @@
         <v>71.74618530273438</v>
       </c>
       <c r="F29" t="n">
-        <v>67.04368591308594</v>
+        <v>67.04367065429688</v>
       </c>
       <c r="G29" t="n">
         <v>46899992</v>
@@ -1136,7 +1136,7 @@
         <v>73.21565246582031</v>
       </c>
       <c r="F31" t="n">
-        <v>68.41682434082031</v>
+        <v>68.41683197021484</v>
       </c>
       <c r="G31" t="n">
         <v>36353548</v>
@@ -1159,7 +1159,7 @@
         <v>76.21183013916016</v>
       </c>
       <c r="F32" t="n">
-        <v>71.21662902832031</v>
+        <v>71.21662139892578</v>
       </c>
       <c r="G32" t="n">
         <v>38263214</v>
@@ -1182,7 +1182,7 @@
         <v>73.56870269775391</v>
       </c>
       <c r="F33" t="n">
-        <v>68.74674224853516</v>
+        <v>68.74673461914062</v>
       </c>
       <c r="G33" t="n">
         <v>47391502</v>
@@ -1205,7 +1205,7 @@
         <v>76.56488800048828</v>
       </c>
       <c r="F34" t="n">
-        <v>71.54654693603516</v>
+        <v>71.54653167724609</v>
       </c>
       <c r="G34" t="n">
         <v>45294665</v>
@@ -1228,7 +1228,7 @@
         <v>77.30915832519531</v>
       </c>
       <c r="F35" t="n">
-        <v>72.24202728271484</v>
+        <v>72.24203491210938</v>
       </c>
       <c r="G35" t="n">
         <v>38546803</v>
@@ -1297,7 +1297,7 @@
         <v>81.72709655761719</v>
       </c>
       <c r="F38" t="n">
-        <v>76.37039947509766</v>
+        <v>76.37040710449219</v>
       </c>
       <c r="G38" t="n">
         <v>38271388</v>
@@ -1343,7 +1343,7 @@
         <v>80.61068725585938</v>
       </c>
       <c r="F40" t="n">
-        <v>75.32715606689453</v>
+        <v>75.32717132568359</v>
       </c>
       <c r="G40" t="n">
         <v>32036731</v>
@@ -1366,7 +1366,7 @@
         <v>81.87976837158203</v>
       </c>
       <c r="F41" t="n">
-        <v>76.5130615234375</v>
+        <v>76.51306915283203</v>
       </c>
       <c r="G41" t="n">
         <v>50181803</v>
@@ -1389,7 +1389,7 @@
         <v>79.13167572021484</v>
       </c>
       <c r="F42" t="n">
-        <v>74.48290252685547</v>
+        <v>74.48291778564453</v>
       </c>
       <c r="G42" t="n">
         <v>40450704</v>
@@ -1458,7 +1458,7 @@
         <v>76.17366027832031</v>
       </c>
       <c r="F45" t="n">
-        <v>71.69866943359375</v>
+        <v>71.69865417480469</v>
       </c>
       <c r="G45" t="n">
         <v>43623732</v>
@@ -1481,7 +1481,7 @@
         <v>76.17366027832031</v>
       </c>
       <c r="F46" t="n">
-        <v>71.69866943359375</v>
+        <v>71.69865417480469</v>
       </c>
       <c r="G46" t="n">
         <v>42834380</v>
@@ -1504,7 +1504,7 @@
         <v>71.76526641845703</v>
       </c>
       <c r="F47" t="n">
-        <v>67.54926300048828</v>
+        <v>67.54925537109375</v>
       </c>
       <c r="G47" t="n">
         <v>50765226</v>
@@ -1573,7 +1573,7 @@
         <v>76.76526641845703</v>
       </c>
       <c r="F50" t="n">
-        <v>72.25550842285156</v>
+        <v>72.25552368164062</v>
       </c>
       <c r="G50" t="n">
         <v>43143331</v>
@@ -1619,7 +1619,7 @@
         <v>78.18701934814453</v>
       </c>
       <c r="F52" t="n">
-        <v>73.59376525878906</v>
+        <v>73.59375</v>
       </c>
       <c r="G52" t="n">
         <v>47570921</v>
@@ -1665,7 +1665,7 @@
         <v>75.88740539550781</v>
       </c>
       <c r="F54" t="n">
-        <v>71.42922973632812</v>
+        <v>71.42922210693359</v>
       </c>
       <c r="G54" t="n">
         <v>77586584</v>
@@ -1711,7 +1711,7 @@
         <v>78.05343627929688</v>
       </c>
       <c r="F56" t="n">
-        <v>74.04817962646484</v>
+        <v>74.04818725585938</v>
       </c>
       <c r="G56" t="n">
         <v>21956754</v>
@@ -1734,7 +1734,7 @@
         <v>79.22709655761719</v>
       </c>
       <c r="F57" t="n">
-        <v>75.16162109375</v>
+        <v>75.16162872314453</v>
       </c>
       <c r="G57" t="n">
         <v>51991595</v>
@@ -1757,7 +1757,7 @@
         <v>79.56106567382812</v>
       </c>
       <c r="F58" t="n">
-        <v>75.47845458984375</v>
+        <v>75.47846221923828</v>
       </c>
       <c r="G58" t="n">
         <v>55280533</v>
@@ -1803,7 +1803,7 @@
         <v>73.54007720947266</v>
       </c>
       <c r="F60" t="n">
-        <v>69.76642608642578</v>
+        <v>69.76641845703125</v>
       </c>
       <c r="G60" t="n">
         <v>57579845</v>
@@ -1826,7 +1826,7 @@
         <v>72.3282470703125</v>
       </c>
       <c r="F61" t="n">
-        <v>68.61678314208984</v>
+        <v>68.61677551269531</v>
       </c>
       <c r="G61" t="n">
         <v>60895507</v>
@@ -1849,7 +1849,7 @@
         <v>71.56488800048828</v>
       </c>
       <c r="F62" t="n">
-        <v>67.89259338378906</v>
+        <v>67.892578125</v>
       </c>
       <c r="G62" t="n">
         <v>57443814</v>
@@ -1918,7 +1918,7 @@
         <v>69.78053283691406</v>
       </c>
       <c r="F65" t="n">
-        <v>66.19980621337891</v>
+        <v>66.19979858398438</v>
       </c>
       <c r="G65" t="n">
         <v>70798478</v>
@@ -1941,7 +1941,7 @@
         <v>71.18320465087891</v>
       </c>
       <c r="F66" t="n">
-        <v>67.53049468994141</v>
+        <v>67.53050231933594</v>
       </c>
       <c r="G66" t="n">
         <v>67107841</v>
@@ -1975,7 +1975,7 @@
         <v>73.95992279052734</v>
       </c>
       <c r="F68" t="n">
-        <v>70.78120422363281</v>
+        <v>70.78119659423828</v>
       </c>
       <c r="G68" t="n">
         <v>123730442</v>
@@ -2021,7 +2021,7 @@
         <v>73.55915832519531</v>
       </c>
       <c r="F70" t="n">
-        <v>70.39766693115234</v>
+        <v>70.39765930175781</v>
       </c>
       <c r="G70" t="n">
         <v>44291520</v>
@@ -2113,7 +2113,7 @@
         <v>71.08778381347656</v>
       </c>
       <c r="F74" t="n">
-        <v>68.03250885009766</v>
+        <v>68.03251647949219</v>
       </c>
       <c r="G74" t="n">
         <v>77213286</v>
@@ -2136,7 +2136,7 @@
         <v>74.81870269775391</v>
       </c>
       <c r="F75" t="n">
-        <v>71.60308074951172</v>
+        <v>71.60307312011719</v>
       </c>
       <c r="G75" t="n">
         <v>64866169</v>
@@ -2159,7 +2159,7 @@
         <v>74.70420074462891</v>
       </c>
       <c r="F76" t="n">
-        <v>71.49349975585938</v>
+        <v>71.49348449707031</v>
       </c>
       <c r="G76" t="n">
         <v>55571144</v>
@@ -2182,7 +2182,7 @@
         <v>75.55343627929688</v>
       </c>
       <c r="F77" t="n">
-        <v>72.30622863769531</v>
+        <v>72.30623626708984</v>
       </c>
       <c r="G77" t="n">
         <v>47817619</v>
@@ -2228,7 +2228,7 @@
         <v>74.11000061035156</v>
       </c>
       <c r="F79" t="n">
-        <v>70.92483520507812</v>
+        <v>70.92481994628906</v>
       </c>
       <c r="G79" t="n">
         <v>56332267</v>
@@ -2262,7 +2262,7 @@
         <v>76.26999664306641</v>
       </c>
       <c r="F81" t="n">
-        <v>72.99198913574219</v>
+        <v>72.99199676513672</v>
       </c>
       <c r="G81" t="n">
         <v>73875900</v>
@@ -2308,7 +2308,7 @@
         <v>77.19999694824219</v>
       </c>
       <c r="F83" t="n">
-        <v>74.51708221435547</v>
+        <v>74.51708984375</v>
       </c>
       <c r="G83" t="n">
         <v>90264500</v>
@@ -2331,7 +2331,7 @@
         <v>78.59999847412109</v>
       </c>
       <c r="F84" t="n">
-        <v>75.86843872070312</v>
+        <v>75.86843109130859</v>
       </c>
       <c r="G84" t="n">
         <v>47184700</v>
@@ -2354,7 +2354,7 @@
         <v>77.98999786376953</v>
       </c>
       <c r="F85" t="n">
-        <v>75.27963256835938</v>
+        <v>75.27962493896484</v>
       </c>
       <c r="G85" t="n">
         <v>29402500</v>
@@ -2423,7 +2423,7 @@
         <v>76.87000274658203</v>
       </c>
       <c r="F88" t="n">
-        <v>74.19855499267578</v>
+        <v>74.19856262207031</v>
       </c>
       <c r="G88" t="n">
         <v>48833200</v>
@@ -2446,7 +2446,7 @@
         <v>75.44000244140625</v>
       </c>
       <c r="F89" t="n">
-        <v>72.81825256347656</v>
+        <v>72.81824493408203</v>
       </c>
       <c r="G89" t="n">
         <v>47301500</v>
@@ -2469,7 +2469,7 @@
         <v>76.72000122070312</v>
       </c>
       <c r="F90" t="n">
-        <v>74.05377197265625</v>
+        <v>74.05376434326172</v>
       </c>
       <c r="G90" t="n">
         <v>38949800</v>
@@ -2515,7 +2515,7 @@
         <v>76.30000305175781</v>
       </c>
       <c r="F92" t="n">
-        <v>73.64836883544922</v>
+        <v>73.64837646484375</v>
       </c>
       <c r="G92" t="n">
         <v>34886900</v>
@@ -2538,7 +2538,7 @@
         <v>77.26000213623047</v>
       </c>
       <c r="F93" t="n">
-        <v>74.57500457763672</v>
+        <v>74.57499694824219</v>
       </c>
       <c r="G93" t="n">
         <v>40665600</v>
@@ -2561,7 +2561,7 @@
         <v>73.44999694824219</v>
       </c>
       <c r="F94" t="n">
-        <v>70.89740753173828</v>
+        <v>70.89739990234375</v>
       </c>
       <c r="G94" t="n">
         <v>47935700</v>
@@ -2641,7 +2641,7 @@
         <v>81.40000152587891</v>
       </c>
       <c r="F98" t="n">
-        <v>79.27526092529297</v>
+        <v>79.2752685546875</v>
       </c>
       <c r="G98" t="n">
         <v>155267200</v>
@@ -2664,7 +2664,7 @@
         <v>80.62999725341797</v>
       </c>
       <c r="F99" t="n">
-        <v>78.52536773681641</v>
+        <v>78.52536010742188</v>
       </c>
       <c r="G99" t="n">
         <v>126450700</v>
@@ -2733,7 +2733,7 @@
         <v>88.05000305175781</v>
       </c>
       <c r="F102" t="n">
-        <v>85.75169372558594</v>
+        <v>85.75168609619141</v>
       </c>
       <c r="G102" t="n">
         <v>74717100</v>
@@ -2802,7 +2802,7 @@
         <v>80.69999694824219</v>
       </c>
       <c r="F105" t="n">
-        <v>78.59352874755859</v>
+        <v>78.59353637695312</v>
       </c>
       <c r="G105" t="n">
         <v>55374400</v>
@@ -2871,7 +2871,7 @@
         <v>72.62000274658203</v>
       </c>
       <c r="F108" t="n">
-        <v>70.72444152832031</v>
+        <v>70.72444915771484</v>
       </c>
       <c r="G108" t="n">
         <v>68810100</v>
@@ -2928,7 +2928,7 @@
         <v>75.73000335693359</v>
       </c>
       <c r="F111" t="n">
-        <v>74.45297241210938</v>
+        <v>74.45298004150391</v>
       </c>
       <c r="G111" t="n">
         <v>45917500</v>
@@ -3135,7 +3135,7 @@
         <v>76.31999969482422</v>
       </c>
       <c r="F120" t="n">
-        <v>75.03302764892578</v>
+        <v>75.03302001953125</v>
       </c>
       <c r="G120" t="n">
         <v>53513100</v>
@@ -3181,7 +3181,7 @@
         <v>78.26000213623047</v>
       </c>
       <c r="F122" t="n">
-        <v>76.9403076171875</v>
+        <v>76.94031524658203</v>
       </c>
       <c r="G122" t="n">
         <v>52335200</v>
@@ -3773,6 +3773,52 @@
         <v>40732300</v>
       </c>
     </row>
+    <row r="149">
+      <c r="A149" s="2" t="n">
+        <v>44809</v>
+      </c>
+      <c r="B149" t="n">
+        <v>86.58000183105469</v>
+      </c>
+      <c r="C149" t="n">
+        <v>88.16999816894531</v>
+      </c>
+      <c r="D149" t="n">
+        <v>85.06999969482422</v>
+      </c>
+      <c r="E149" t="n">
+        <v>87.33999633789062</v>
+      </c>
+      <c r="F149" t="n">
+        <v>87.33999633789062</v>
+      </c>
+      <c r="G149" t="n">
+        <v>29955300</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="2" t="n">
+        <v>44813</v>
+      </c>
+      <c r="B150" t="n">
+        <v>87.58999633789062</v>
+      </c>
+      <c r="C150" t="n">
+        <v>88.15499877929688</v>
+      </c>
+      <c r="D150" t="n">
+        <v>87.26999664306641</v>
+      </c>
+      <c r="E150" t="n">
+        <v>87.33999633789062</v>
+      </c>
+      <c r="F150" t="n">
+        <v>87.33999633789062</v>
+      </c>
+      <c r="G150" t="n">
+        <v>7481322</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
performance report testing created
</commit_message>
<xml_diff>
--- a/Excel reports/mrk_raw_dataset.xlsx
+++ b/Excel reports/mrk_raw_dataset.xlsx
@@ -585,7 +585,7 @@
         <v>81.52671813964844</v>
       </c>
       <c r="F6" t="n">
-        <v>74.36357116699219</v>
+        <v>74.36360168457031</v>
       </c>
       <c r="G6" t="n">
         <v>49493162</v>
@@ -608,7 +608,7 @@
         <v>81.18320465087891</v>
       </c>
       <c r="F7" t="n">
-        <v>74.05024719238281</v>
+        <v>74.05026245117188</v>
       </c>
       <c r="G7" t="n">
         <v>81640353</v>
@@ -654,7 +654,7 @@
         <v>78.56870269775391</v>
       </c>
       <c r="F9" t="n">
-        <v>71.66546630859375</v>
+        <v>71.66545104980469</v>
       </c>
       <c r="G9" t="n">
         <v>41994828</v>
@@ -677,7 +677,7 @@
         <v>73.05343627929688</v>
       </c>
       <c r="F10" t="n">
-        <v>66.63479614257812</v>
+        <v>66.63478851318359</v>
       </c>
       <c r="G10" t="n">
         <v>83826481</v>
@@ -757,7 +757,7 @@
         <v>68.09160614013672</v>
       </c>
       <c r="F14" t="n">
-        <v>62.62199783325195</v>
+        <v>62.62200164794922</v>
       </c>
       <c r="G14" t="n">
         <v>106457307</v>
@@ -780,7 +780,7 @@
         <v>68.44465637207031</v>
       </c>
       <c r="F15" t="n">
-        <v>62.94670104980469</v>
+        <v>62.94669342041016</v>
       </c>
       <c r="G15" t="n">
         <v>87108502</v>
@@ -826,7 +826,7 @@
         <v>78.71183013916016</v>
       </c>
       <c r="F17" t="n">
-        <v>72.38914489746094</v>
+        <v>72.38913726806641</v>
       </c>
       <c r="G17" t="n">
         <v>50330514</v>
@@ -918,7 +918,7 @@
         <v>72.90076446533203</v>
       </c>
       <c r="F21" t="n">
-        <v>67.04486846923828</v>
+        <v>67.04486083984375</v>
       </c>
       <c r="G21" t="n">
         <v>50060654</v>
@@ -941,7 +941,7 @@
         <v>76.12595367431641</v>
       </c>
       <c r="F22" t="n">
-        <v>70.01095581054688</v>
+        <v>70.01097869873047</v>
       </c>
       <c r="G22" t="n">
         <v>51877153</v>
@@ -964,7 +964,7 @@
         <v>72.87213897705078</v>
       </c>
       <c r="F23" t="n">
-        <v>67.01853179931641</v>
+        <v>67.01853942871094</v>
       </c>
       <c r="G23" t="n">
         <v>49529948</v>
@@ -987,7 +987,7 @@
         <v>77.02290344238281</v>
       </c>
       <c r="F24" t="n">
-        <v>70.83587646484375</v>
+        <v>70.83586883544922</v>
       </c>
       <c r="G24" t="n">
         <v>58673014</v>
@@ -1033,7 +1033,7 @@
         <v>72.80534362792969</v>
       </c>
       <c r="F26" t="n">
-        <v>66.95709228515625</v>
+        <v>66.95710754394531</v>
       </c>
       <c r="G26" t="n">
         <v>59188420</v>
@@ -1067,7 +1067,7 @@
         <v>74.33206176757812</v>
       </c>
       <c r="F28" t="n">
-        <v>68.90458679199219</v>
+        <v>68.90456390380859</v>
       </c>
       <c r="G28" t="n">
         <v>78546553</v>
@@ -1090,7 +1090,7 @@
         <v>71.74618530273438</v>
       </c>
       <c r="F29" t="n">
-        <v>66.50752258300781</v>
+        <v>66.50750732421875</v>
       </c>
       <c r="G29" t="n">
         <v>46899992</v>
@@ -1113,7 +1113,7 @@
         <v>75.1717529296875</v>
       </c>
       <c r="F30" t="n">
-        <v>69.68295288085938</v>
+        <v>69.68296051025391</v>
       </c>
       <c r="G30" t="n">
         <v>33948388</v>
@@ -1159,7 +1159,7 @@
         <v>76.21183013916016</v>
       </c>
       <c r="F32" t="n">
-        <v>70.6470947265625</v>
+        <v>70.64708709716797</v>
       </c>
       <c r="G32" t="n">
         <v>38263214</v>
@@ -1182,7 +1182,7 @@
         <v>73.56870269775391</v>
       </c>
       <c r="F33" t="n">
-        <v>68.19696044921875</v>
+        <v>68.19695281982422</v>
       </c>
       <c r="G33" t="n">
         <v>47391502</v>
@@ -1205,7 +1205,7 @@
         <v>76.56488800048828</v>
       </c>
       <c r="F34" t="n">
-        <v>70.97438049316406</v>
+        <v>70.974365234375</v>
       </c>
       <c r="G34" t="n">
         <v>45294665</v>
@@ -1228,7 +1228,7 @@
         <v>77.30915832519531</v>
       </c>
       <c r="F35" t="n">
-        <v>71.664306640625</v>
+        <v>71.66429901123047</v>
       </c>
       <c r="G35" t="n">
         <v>38546803</v>
@@ -1251,7 +1251,7 @@
         <v>79.65648651123047</v>
       </c>
       <c r="F36" t="n">
-        <v>73.84023284912109</v>
+        <v>73.84022521972656</v>
       </c>
       <c r="G36" t="n">
         <v>35560526</v>
@@ -1297,7 +1297,7 @@
         <v>81.72709655761719</v>
       </c>
       <c r="F38" t="n">
-        <v>75.75965118408203</v>
+        <v>75.7596435546875</v>
       </c>
       <c r="G38" t="n">
         <v>38271388</v>
@@ -1366,7 +1366,7 @@
         <v>81.87976837158203</v>
       </c>
       <c r="F41" t="n">
-        <v>75.90116882324219</v>
+        <v>75.90117645263672</v>
       </c>
       <c r="G41" t="n">
         <v>50181803</v>
@@ -1389,7 +1389,7 @@
         <v>79.13167572021484</v>
       </c>
       <c r="F42" t="n">
-        <v>73.88724517822266</v>
+        <v>73.88725280761719</v>
       </c>
       <c r="G42" t="n">
         <v>40450704</v>
@@ -1504,7 +1504,7 @@
         <v>71.76526641845703</v>
       </c>
       <c r="F47" t="n">
-        <v>67.00904846191406</v>
+        <v>67.00905609130859</v>
       </c>
       <c r="G47" t="n">
         <v>50765226</v>
@@ -1550,7 +1550,7 @@
         <v>77.37595367431641</v>
       </c>
       <c r="F49" t="n">
-        <v>72.24790191650391</v>
+        <v>72.24788665771484</v>
       </c>
       <c r="G49" t="n">
         <v>40678643</v>
@@ -1619,7 +1619,7 @@
         <v>78.18701934814453</v>
       </c>
       <c r="F52" t="n">
-        <v>73.00520324707031</v>
+        <v>73.00521087646484</v>
       </c>
       <c r="G52" t="n">
         <v>47570921</v>
@@ -1665,7 +1665,7 @@
         <v>75.88740539550781</v>
       </c>
       <c r="F54" t="n">
-        <v>70.85800170898438</v>
+        <v>70.85799407958984</v>
       </c>
       <c r="G54" t="n">
         <v>77586584</v>
@@ -1688,7 +1688,7 @@
         <v>76.46946716308594</v>
       </c>
       <c r="F55" t="n">
-        <v>71.96534729003906</v>
+        <v>71.96533966064453</v>
       </c>
       <c r="G55" t="n">
         <v>29206712</v>
@@ -1734,7 +1734,7 @@
         <v>79.22709655761719</v>
       </c>
       <c r="F57" t="n">
-        <v>74.56053161621094</v>
+        <v>74.560546875</v>
       </c>
       <c r="G57" t="n">
         <v>51991595</v>
@@ -1780,7 +1780,7 @@
         <v>77.27098846435547</v>
       </c>
       <c r="F59" t="n">
-        <v>72.71965026855469</v>
+        <v>72.71964263916016</v>
       </c>
       <c r="G59" t="n">
         <v>38045859</v>
@@ -1803,7 +1803,7 @@
         <v>73.54007720947266</v>
       </c>
       <c r="F60" t="n">
-        <v>69.20848846435547</v>
+        <v>69.20848083496094</v>
       </c>
       <c r="G60" t="n">
         <v>57579845</v>
@@ -1826,7 +1826,7 @@
         <v>72.3282470703125</v>
       </c>
       <c r="F61" t="n">
-        <v>68.06803131103516</v>
+        <v>68.06803894042969</v>
       </c>
       <c r="G61" t="n">
         <v>60895507</v>
@@ -1849,7 +1849,7 @@
         <v>71.56488800048828</v>
       </c>
       <c r="F62" t="n">
-        <v>67.34964752197266</v>
+        <v>67.34963226318359</v>
       </c>
       <c r="G62" t="n">
         <v>57443814</v>
@@ -1872,7 +1872,7 @@
         <v>70.90648651123047</v>
       </c>
       <c r="F63" t="n">
-        <v>66.73001861572266</v>
+        <v>66.73003387451172</v>
       </c>
       <c r="G63" t="n">
         <v>46003741</v>
@@ -1895,7 +1895,7 @@
         <v>69.29389190673828</v>
       </c>
       <c r="F64" t="n">
-        <v>65.21240234375</v>
+        <v>65.21240997314453</v>
       </c>
       <c r="G64" t="n">
         <v>57903573</v>
@@ -1941,7 +1941,7 @@
         <v>71.18320465087891</v>
       </c>
       <c r="F66" t="n">
-        <v>66.99043273925781</v>
+        <v>66.99044036865234</v>
       </c>
       <c r="G66" t="n">
         <v>67107841</v>
@@ -1975,7 +1975,7 @@
         <v>73.95992279052734</v>
       </c>
       <c r="F68" t="n">
-        <v>70.21515655517578</v>
+        <v>70.21514129638672</v>
       </c>
       <c r="G68" t="n">
         <v>123730442</v>
@@ -2021,7 +2021,7 @@
         <v>73.55915832519531</v>
       </c>
       <c r="F70" t="n">
-        <v>69.83467864990234</v>
+        <v>69.83468627929688</v>
       </c>
       <c r="G70" t="n">
         <v>44291520</v>
@@ -2044,7 +2044,7 @@
         <v>72.81488800048828</v>
       </c>
       <c r="F71" t="n">
-        <v>69.12808990478516</v>
+        <v>69.12809753417969</v>
       </c>
       <c r="G71" t="n">
         <v>52378831</v>
@@ -2159,7 +2159,7 @@
         <v>74.70420074462891</v>
       </c>
       <c r="F76" t="n">
-        <v>70.9217529296875</v>
+        <v>70.92174530029297</v>
       </c>
       <c r="G76" t="n">
         <v>55571144</v>
@@ -2182,7 +2182,7 @@
         <v>75.55343627929688</v>
       </c>
       <c r="F77" t="n">
-        <v>71.72798156738281</v>
+        <v>71.72797393798828</v>
       </c>
       <c r="G77" t="n">
         <v>47817619</v>
@@ -2285,7 +2285,7 @@
         <v>76.61000061035156</v>
       </c>
       <c r="F82" t="n">
-        <v>72.73105621337891</v>
+        <v>72.73104858398438</v>
       </c>
       <c r="G82" t="n">
         <v>73189100</v>
@@ -2308,7 +2308,7 @@
         <v>77.19999694824219</v>
       </c>
       <c r="F83" t="n">
-        <v>73.92115783691406</v>
+        <v>73.92115020751953</v>
       </c>
       <c r="G83" t="n">
         <v>90264500</v>
@@ -2331,7 +2331,7 @@
         <v>78.59999847412109</v>
       </c>
       <c r="F84" t="n">
-        <v>75.26168823242188</v>
+        <v>75.26169586181641</v>
       </c>
       <c r="G84" t="n">
         <v>47184700</v>
@@ -2423,7 +2423,7 @@
         <v>76.87000274658203</v>
       </c>
       <c r="F88" t="n">
-        <v>73.60517883300781</v>
+        <v>73.60517120361328</v>
       </c>
       <c r="G88" t="n">
         <v>48833200</v>
@@ -2584,7 +2584,7 @@
         <v>71.68000030517578</v>
       </c>
       <c r="F95" t="n">
-        <v>68.63559722900391</v>
+        <v>68.63560485839844</v>
       </c>
       <c r="G95" t="n">
         <v>97229400</v>
@@ -2618,7 +2618,7 @@
         <v>73.61000061035156</v>
       </c>
       <c r="F97" t="n">
-        <v>71.11528778076172</v>
+        <v>71.11529541015625</v>
       </c>
       <c r="G97" t="n">
         <v>64542200</v>
@@ -2641,7 +2641,7 @@
         <v>81.40000152587891</v>
       </c>
       <c r="F98" t="n">
-        <v>78.64128112792969</v>
+        <v>78.64128875732422</v>
       </c>
       <c r="G98" t="n">
         <v>155267200</v>
@@ -2687,7 +2687,7 @@
         <v>78.33000183105469</v>
       </c>
       <c r="F100" t="n">
-        <v>75.67533111572266</v>
+        <v>75.67532348632812</v>
       </c>
       <c r="G100" t="n">
         <v>59162000</v>
@@ -2802,7 +2802,7 @@
         <v>80.69999694824219</v>
       </c>
       <c r="F105" t="n">
-        <v>77.96500396728516</v>
+        <v>77.96499633789062</v>
       </c>
       <c r="G105" t="n">
         <v>55374400</v>
@@ -2825,7 +2825,7 @@
         <v>79.16000366210938</v>
       </c>
       <c r="F106" t="n">
-        <v>76.47720336914062</v>
+        <v>76.47719573974609</v>
       </c>
       <c r="G106" t="n">
         <v>49570000</v>
@@ -2848,7 +2848,7 @@
         <v>73.33999633789062</v>
       </c>
       <c r="F107" t="n">
-        <v>70.85444641113281</v>
+        <v>70.85443878173828</v>
       </c>
       <c r="G107" t="n">
         <v>115662400</v>
@@ -2871,7 +2871,7 @@
         <v>72.62000274658203</v>
       </c>
       <c r="F108" t="n">
-        <v>70.15885925292969</v>
+        <v>70.15884399414062</v>
       </c>
       <c r="G108" t="n">
         <v>68810100</v>
@@ -2894,7 +2894,7 @@
         <v>75.69000244140625</v>
       </c>
       <c r="F109" t="n">
-        <v>73.12480163574219</v>
+        <v>73.12479400634766</v>
       </c>
       <c r="G109" t="n">
         <v>95341500</v>
@@ -2928,7 +2928,7 @@
         <v>75.73000335693359</v>
       </c>
       <c r="F111" t="n">
-        <v>73.85756683349609</v>
+        <v>73.85755920410156</v>
       </c>
       <c r="G111" t="n">
         <v>45917500</v>
@@ -2951,7 +2951,7 @@
         <v>76.63999938964844</v>
       </c>
       <c r="F112" t="n">
-        <v>74.74505615234375</v>
+        <v>74.74504852294922</v>
       </c>
       <c r="G112" t="n">
         <v>29866500</v>
@@ -3020,7 +3020,7 @@
         <v>79.98000335693359</v>
       </c>
       <c r="F115" t="n">
-        <v>78.00247955322266</v>
+        <v>78.00247192382812</v>
       </c>
       <c r="G115" t="n">
         <v>56472600</v>
@@ -3066,7 +3066,7 @@
         <v>78.55999755859375</v>
       </c>
       <c r="F117" t="n">
-        <v>76.61757659912109</v>
+        <v>76.61758422851562</v>
       </c>
       <c r="G117" t="n">
         <v>67724100</v>
@@ -3089,7 +3089,7 @@
         <v>76.63999938964844</v>
       </c>
       <c r="F118" t="n">
-        <v>74.74505615234375</v>
+        <v>74.74504852294922</v>
       </c>
       <c r="G118" t="n">
         <v>78064800</v>
@@ -3250,7 +3250,7 @@
         <v>83.51999664306641</v>
       </c>
       <c r="F125" t="n">
-        <v>82.17950439453125</v>
+        <v>82.17949676513672</v>
       </c>
       <c r="G125" t="n">
         <v>46350700</v>
@@ -3273,7 +3273,7 @@
         <v>87.68000030517578</v>
       </c>
       <c r="F126" t="n">
-        <v>86.27273559570312</v>
+        <v>86.27274322509766</v>
       </c>
       <c r="G126" t="n">
         <v>59518400</v>
@@ -3296,7 +3296,7 @@
         <v>86.91000366210938</v>
       </c>
       <c r="F127" t="n">
-        <v>85.51510620117188</v>
+        <v>85.51509857177734</v>
       </c>
       <c r="G127" t="n">
         <v>61763900</v>
@@ -3388,7 +3388,7 @@
         <v>90.41000366210938</v>
       </c>
       <c r="F131" t="n">
-        <v>88.95893096923828</v>
+        <v>88.95892333984375</v>
       </c>
       <c r="G131" t="n">
         <v>65129200</v>

</xml_diff>